<commit_message>
Fund formula uppdate only (#1073)
* Added update only to import fund formula

* Formulas Update assigns sequence properly

* Added scenario to fund ratio download

* review changes in formulas import

* Minor comment and return value fix

* Fixed import formulas and specs, updated True false columns to Yes No

* Remove debugger from spec

* Update import fund formulas to be simpler
</commit_message>
<xml_diff>
--- a/public/sample_uploads/allocate_account_entries/fund_formulas.xlsx
+++ b/public/sample_uploads/allocate_account_entries/fund_formulas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="140">
   <si>
     <t xml:space="preserve">Sequence</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">Capital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
   </si>
   <si>
     <t xml:space="preserve">Foreign Commitment</t>
@@ -170,9 +173,6 @@
   </si>
   <si>
     <t xml:space="preserve">Management Fees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
   </si>
   <si>
     <t xml:space="preserve">capital_commitment.committed_amount_cents * ( fund_unit_setting.management_fee * ( (@end_date - @start_date ).to_i  + 1 ) / 365 ) / 100</t>
@@ -458,8 +458,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -526,12 +527,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -734,11 +739,11 @@
   </sheetPr>
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="F34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G59" activeCellId="0" sqref="G59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.75"/>
@@ -787,7 +792,7 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -813,13 +818,11 @@
       <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,7 +830,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
@@ -839,18 +842,16 @@
         <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -858,10 +859,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
@@ -870,18 +871,16 @@
         <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -889,7 +888,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -901,18 +900,16 @@
         <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -920,10 +917,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>14</v>
@@ -932,18 +929,16 @@
         <v>15</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -951,7 +946,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -963,18 +958,16 @@
         <v>15</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -982,7 +975,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -994,18 +987,16 @@
         <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,7 +1004,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -1025,18 +1016,16 @@
         <v>15</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1044,10 +1033,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>14</v>
@@ -1056,18 +1045,16 @@
         <v>15</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,10 +1062,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>14</v>
@@ -1087,18 +1074,16 @@
         <v>15</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1106,30 +1091,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,30 +1120,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J13" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1168,61 +1149,57 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="48.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J15" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K15" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,7 +1207,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1239,21 +1216,19 @@
         <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>50</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J16" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1267,7 +1242,7 @@
         <v>13</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>15</v>
@@ -1278,13 +1253,11 @@
       <c r="H17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J17" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1298,7 +1271,7 @@
         <v>13</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>15</v>
@@ -1309,13 +1282,11 @@
       <c r="H18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J18" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K18" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1329,7 +1300,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>15</v>
@@ -1340,13 +1311,11 @@
       <c r="H19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J19" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K19" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1360,7 +1329,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>15</v>
@@ -1371,13 +1340,11 @@
       <c r="H20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J20" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K20" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1391,7 +1358,7 @@
         <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>15</v>
@@ -1402,13 +1369,11 @@
       <c r="H21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K21" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1422,7 +1387,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>15</v>
@@ -1433,13 +1398,11 @@
       <c r="H22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J22" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K22" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1464,13 +1427,11 @@
       <c r="H23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K23" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1484,7 +1445,7 @@
         <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>15</v>
@@ -1495,13 +1456,11 @@
       <c r="H24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1515,7 +1474,7 @@
         <v>13</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>15</v>
@@ -1526,13 +1485,11 @@
       <c r="H25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K25" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1543,7 +1500,7 @@
         <v>70</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>14</v>
@@ -1552,18 +1509,16 @@
         <v>15</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K26" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1577,7 +1532,7 @@
         <v>13</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>15</v>
@@ -1588,13 +1543,11 @@
       <c r="H27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K27" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1608,7 +1561,7 @@
         <v>13</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>15</v>
@@ -1619,13 +1572,11 @@
       <c r="H28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K28" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1639,7 +1590,7 @@
         <v>13</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>15</v>
@@ -1650,16 +1601,14 @@
       <c r="H29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J29" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K29" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
@@ -1673,24 +1622,22 @@
         <v>14</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>79</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J30" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K30" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
@@ -1706,19 +1653,17 @@
       <c r="E31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="3" t="s">
         <v>79</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J31" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K31" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1741,15 +1686,13 @@
         <v>80</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J32" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K32" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1763,7 +1706,7 @@
         <v>13</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>15</v>
@@ -1772,15 +1715,13 @@
         <v>84</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J33" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K33" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1794,7 +1735,7 @@
         <v>13</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>15</v>
@@ -1803,15 +1744,13 @@
         <v>86</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J34" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K34" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1825,7 +1764,7 @@
         <v>13</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>15</v>
@@ -1834,18 +1773,16 @@
         <v>88</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J35" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K35" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>35</v>
       </c>
@@ -1861,22 +1798,20 @@
       <c r="E36" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="3" t="s">
         <v>79</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J36" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K36" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
         <v>36</v>
       </c>
@@ -1884,7 +1819,7 @@
         <v>91</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>14</v>
@@ -1892,19 +1827,17 @@
       <c r="E37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="3" t="s">
         <v>79</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J37" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K37" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1918,7 +1851,7 @@
         <v>13</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>15</v>
@@ -1929,13 +1862,11 @@
       <c r="H38" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J38" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K38" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1949,7 +1880,7 @@
         <v>13</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>15</v>
@@ -1960,13 +1891,11 @@
       <c r="H39" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J39" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K39" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,7 +1909,7 @@
         <v>13</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>15</v>
@@ -1991,13 +1920,11 @@
       <c r="H40" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J40" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K40" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2011,7 +1938,7 @@
         <v>13</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>15</v>
@@ -2022,13 +1949,11 @@
       <c r="H41" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J41" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K41" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2042,7 +1967,7 @@
         <v>13</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>15</v>
@@ -2053,16 +1978,14 @@
       <c r="H42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J42" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K42" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <v>42</v>
       </c>
@@ -2073,24 +1996,22 @@
         <v>13</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="3" t="s">
         <v>103</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J43" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K43" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2104,7 +2025,7 @@
         <v>13</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>15</v>
@@ -2115,13 +2036,11 @@
       <c r="H44" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J44" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K44" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="J44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2135,7 +2054,7 @@
         <v>13</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>15</v>
@@ -2146,16 +2065,14 @@
       <c r="H45" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J45" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K45" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="48.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J45" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
         <v>45</v>
       </c>
@@ -2163,30 +2080,28 @@
         <v>108</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G46" s="3" t="s">
         <v>109</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J46" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K46" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="48.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
         <v>46</v>
       </c>
@@ -2194,27 +2109,25 @@
         <v>110</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G47" s="3" t="s">
         <v>111</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J47" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K47" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2228,7 +2141,7 @@
         <v>113</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>15</v>
@@ -2237,15 +2150,13 @@
         <v>114</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J48" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K48" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2253,13 +2164,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>15</v>
@@ -2268,46 +2179,42 @@
         <v>115</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J49" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K49" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="G50" s="3" t="s">
         <v>116</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J50" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K50" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2315,13 +2222,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>15</v>
@@ -2330,15 +2237,13 @@
         <v>117</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J51" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K51" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2346,13 +2251,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>118</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>15</v>
@@ -2361,15 +2266,13 @@
         <v>119</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J52" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K52" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2380,10 +2283,10 @@
         <v>120</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>15</v>
@@ -2392,15 +2295,13 @@
         <v>121</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J53" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K53" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2411,10 +2312,10 @@
         <v>122</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>15</v>
@@ -2423,15 +2324,13 @@
         <v>123</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J54" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K54" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2454,15 +2353,13 @@
         <v>125</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J55" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K55" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2481,19 +2378,17 @@
       <c r="E56" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="G56" s="4" t="s">
         <v>127</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J56" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K56" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2512,19 +2407,17 @@
       <c r="E57" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="G57" s="4" t="s">
         <v>129</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J57" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K57" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2543,19 +2436,17 @@
       <c r="E58" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G58" s="3" t="s">
+      <c r="G58" s="4" t="s">
         <v>131</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J58" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K58" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2578,15 +2469,13 @@
         <v>134</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J59" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K59" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2609,15 +2498,13 @@
         <v>136</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J60" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K60" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2631,7 +2518,7 @@
         <v>138</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>15</v>
@@ -2640,15 +2527,13 @@
         <v>139</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J61" s="1" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K61" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>